<commit_message>
Last fixes before exam
</commit_message>
<xml_diff>
--- a/Assignments/A04/Multiclass+data.xlsx
+++ b/Assignments/A04/Multiclass+data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gribaudo/Documents/Corsi/2021/CSPE/Exercise session/Assignments/A04/Pub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Polimi\2020-computer-systems-performance-evaluation\Assignments\A04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8FE78E-8336-AC46-998A-E640DC588BBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F849924-BE12-4519-9523-F5CBCF8B4239}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30360" yWindow="3580" windowWidth="25440" windowHeight="14240" xr2:uid="{9512203D-D33A-624C-A353-928C45FEB173}"/>
+    <workbookView xWindow="-20617" yWindow="-98" windowWidth="20715" windowHeight="13425" xr2:uid="{9512203D-D33A-624C-A353-928C45FEB173}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,19 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Data!$A$1:$S$24</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1030,7 +1039,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1046,7 +1055,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1347,19 +1356,19 @@
   </sheetPr>
   <dimension ref="A1:AK27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:AB25"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AF8" sqref="AF8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="6.1640625" style="1" customWidth="1"/>
+    <col min="1" max="5" width="6.125" style="1" customWidth="1"/>
     <col min="7" max="17" width="6.5" customWidth="1"/>
-    <col min="18" max="18" width="10.33203125" customWidth="1"/>
-    <col min="30" max="30" width="23.6640625" customWidth="1"/>
+    <col min="18" max="18" width="10.375" customWidth="1"/>
+    <col min="30" max="30" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="65"/>
       <c r="B1" s="66"/>
       <c r="C1" s="66"/>
@@ -1399,7 +1408,7 @@
       </c>
       <c r="AB1" s="57"/>
     </row>
-    <row r="2" spans="1:37" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="65" t="s">
         <v>2</v>
       </c>
@@ -1447,7 +1456,7 @@
       <c r="AA2" s="41"/>
       <c r="AB2" s="13"/>
     </row>
-    <row r="3" spans="1:37" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="68" t="s">
         <v>0</v>
       </c>
@@ -1528,7 +1537,7 @@
         <v>20</v>
       </c>
       <c r="AE3" s="39">
-        <v>10000051</v>
+        <v>10566859</v>
       </c>
       <c r="AF3" t="s">
         <v>21</v>
@@ -1537,7 +1546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>0</v>
       </c>
@@ -1624,10 +1633,10 @@
       </c>
       <c r="AK4">
         <f>MOD(AE3,20)+AK3</f>
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -1720,13 +1729,13 @@
       </c>
       <c r="AF5" s="40">
         <f ca="1">INDIRECT($AK5&amp;AK$4)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AK5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2</v>
       </c>
@@ -1822,7 +1831,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -1921,7 +1930,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>4</v>
       </c>
@@ -2014,13 +2023,13 @@
       </c>
       <c r="AF8" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AK8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>5</v>
       </c>
@@ -2110,13 +2119,13 @@
       </c>
       <c r="AF9" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
+        <v>0.4</v>
       </c>
       <c r="AK9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>6</v>
       </c>
@@ -2206,13 +2215,13 @@
       </c>
       <c r="AF10" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5</v>
+        <v>0.2</v>
       </c>
       <c r="AK10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>7</v>
       </c>
@@ -2302,13 +2311,13 @@
       </c>
       <c r="AF11" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="AK11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>8</v>
       </c>
@@ -2398,13 +2407,13 @@
       </c>
       <c r="AF12" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="AK12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>9</v>
       </c>
@@ -2494,13 +2503,13 @@
       </c>
       <c r="AF13" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="AK13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>10</v>
       </c>
@@ -2590,13 +2599,13 @@
       </c>
       <c r="AF14" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AK14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>11</v>
       </c>
@@ -2686,13 +2695,13 @@
       </c>
       <c r="AF15" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="AK15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>12</v>
       </c>
@@ -2782,13 +2791,13 @@
       </c>
       <c r="AF16" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AK16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>13</v>
       </c>
@@ -2881,13 +2890,13 @@
       </c>
       <c r="AF17" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>0.09</v>
+        <v>0.8</v>
       </c>
       <c r="AK17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>14</v>
       </c>
@@ -2977,13 +2986,13 @@
       </c>
       <c r="AF18" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="AK18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>15</v>
       </c>
@@ -3073,13 +3082,13 @@
       </c>
       <c r="AF19" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AK19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>16</v>
       </c>
@@ -3169,13 +3178,13 @@
       </c>
       <c r="AF20" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0.74999999999999989</v>
       </c>
       <c r="AK20" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>17</v>
       </c>
@@ -3265,13 +3274,13 @@
       </c>
       <c r="AF21" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AK21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>18</v>
       </c>
@@ -3367,7 +3376,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:37" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>19</v>
       </c>
@@ -3457,13 +3466,13 @@
       </c>
       <c r="AF23" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15833333333333333</v>
+        <v>0.31666666666666665</v>
       </c>
       <c r="AK23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="62" t="s">
         <v>18</v>
       </c>
@@ -3545,13 +3554,13 @@
       </c>
       <c r="AF24" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AK24" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="53" t="s">
         <v>19</v>
       </c>
@@ -3633,13 +3642,13 @@
       </c>
       <c r="AF25" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AK25" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AD26" t="s">
         <v>5</v>
       </c>
@@ -3654,7 +3663,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AE27" t="s">
         <v>53</v>
       </c>

</xml_diff>